<commit_message>
Adicao do Botao de Graficos (ainda nao funciona)
</commit_message>
<xml_diff>
--- a/tabela-excel/amostras.xlsx
+++ b/tabela-excel/amostras.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,6 +823,1095 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>101024ac</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2.013</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3427</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2.307</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6182</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2.622</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>4405</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2.957</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>26535</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>310</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3.313</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>103432</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>363</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>3.691</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>13307</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>4.509</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>347</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>5.412</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>842</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>5.895</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2593</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>6.399</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>173</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>6.925</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2247</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>7.472</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1849</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>238</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>8.041</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>1538</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>8.631</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2394</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>251</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2.984</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>18767</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>101024ad</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2.013</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2996</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2.307</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>5715</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2.622</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>4051</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2.957</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>24452</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>302</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>3.313</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>99485</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>356</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>3.691</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>13408</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>4.509</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>370</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>5.412</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>823</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>5.895</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2506</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>6.399</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>12580</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>6.925</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2424</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>161</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>7.472</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2408</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>273</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>8.041</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2337</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>282</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>8.631</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>3741</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2.984</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>18132</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>199</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>101024ae</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2.013</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2490</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2.307</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>5127</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2.622</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>3703</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2.957</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>21646</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>282</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>3.313</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>80536</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>323</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>3.691</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>11741</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>168</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>4.509</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>459</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>5.412</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>811</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>5.895</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>1972</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>6.399</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>9505</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>163</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>6.925</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>1982</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>7.472</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>1803</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>225</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>8.041</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>1639</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>237</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>8.631</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2331</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2.984</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>15420</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -835,7 +1924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -916,6 +2005,99 @@
         <v>35.9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>101024ac</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2059.808</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11.919</v>
+      </c>
+      <c r="D3" t="n">
+        <v>145.486</v>
+      </c>
+      <c r="E3" t="n">
+        <v>17660.927</v>
+      </c>
+      <c r="F3" t="n">
+        <v>31.016</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5081.724</v>
+      </c>
+      <c r="H3" t="n">
+        <v>238.826</v>
+      </c>
+      <c r="I3" t="n">
+        <v>32.349</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>101024ad</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2252.243</v>
+      </c>
+      <c r="C4" t="n">
+        <v>19.654</v>
+      </c>
+      <c r="D4" t="n">
+        <v>191.563</v>
+      </c>
+      <c r="E4" t="n">
+        <v>18434.055</v>
+      </c>
+      <c r="F4" t="n">
+        <v>32.529</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4821.07</v>
+      </c>
+      <c r="H4" t="n">
+        <v>239.592</v>
+      </c>
+      <c r="I4" t="n">
+        <v>54.856</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>101024ae</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2227.886</v>
+      </c>
+      <c r="C5" t="n">
+        <v>15.57</v>
+      </c>
+      <c r="D5" t="n">
+        <v>163.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>16857.379</v>
+      </c>
+      <c r="F5" t="n">
+        <v>28.916</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4526.242</v>
+      </c>
+      <c r="H5" t="n">
+        <v>242.805</v>
+      </c>
+      <c r="I5" t="n">
+        <v>38.611</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de dados na tela em tempo real.
</commit_message>
<xml_diff>
--- a/tabela-excel/amostras.xlsx
+++ b/tabela-excel/amostras.xlsx
@@ -1924,7 +1924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1940,37 +1940,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cu</t>
+          <t>K</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Fe</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Mn</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Zn</t>
+          <t>Ti</t>
         </is>
       </c>
     </row>
@@ -1981,28 +1956,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2022</v>
+        <v>25925.248</v>
       </c>
       <c r="C2" t="n">
-        <v>12.8</v>
+        <v>20124.517</v>
       </c>
       <c r="D2" t="n">
-        <v>137</v>
-      </c>
-      <c r="E2" t="n">
-        <v>17762</v>
-      </c>
-      <c r="F2" t="n">
-        <v>32.6</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5250</v>
-      </c>
-      <c r="H2" t="n">
-        <v>258</v>
-      </c>
-      <c r="I2" t="n">
-        <v>35.9</v>
+        <v>6412.352</v>
       </c>
     </row>
     <row r="3">
@@ -2012,28 +1972,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2059.808</v>
+        <v>26410</v>
       </c>
       <c r="C3" t="n">
-        <v>11.919</v>
+        <v>20010</v>
       </c>
       <c r="D3" t="n">
-        <v>145.486</v>
-      </c>
-      <c r="E3" t="n">
-        <v>17660.927</v>
-      </c>
-      <c r="F3" t="n">
-        <v>31.016</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5081.724</v>
-      </c>
-      <c r="H3" t="n">
-        <v>238.826</v>
-      </c>
-      <c r="I3" t="n">
-        <v>32.349</v>
+        <v>4570</v>
       </c>
     </row>
     <row r="4">
@@ -2043,28 +1988,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2252.243</v>
+        <v>28877.324</v>
       </c>
       <c r="C4" t="n">
-        <v>19.654</v>
+        <v>20885.962</v>
       </c>
       <c r="D4" t="n">
-        <v>191.563</v>
-      </c>
-      <c r="E4" t="n">
-        <v>18434.055</v>
-      </c>
-      <c r="F4" t="n">
-        <v>32.529</v>
-      </c>
-      <c r="G4" t="n">
-        <v>4821.07</v>
-      </c>
-      <c r="H4" t="n">
-        <v>239.592</v>
-      </c>
-      <c r="I4" t="n">
-        <v>54.856</v>
+        <v>5288.021</v>
       </c>
     </row>
     <row r="5">
@@ -2074,28 +2004,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2227.886</v>
+        <v>28565.036</v>
       </c>
       <c r="C5" t="n">
-        <v>15.57</v>
+        <v>19099.573</v>
       </c>
       <c r="D5" t="n">
-        <v>163.5</v>
-      </c>
-      <c r="E5" t="n">
-        <v>16857.379</v>
-      </c>
-      <c r="F5" t="n">
-        <v>28.916</v>
-      </c>
-      <c r="G5" t="n">
-        <v>4526.242</v>
-      </c>
-      <c r="H5" t="n">
-        <v>242.805</v>
-      </c>
-      <c r="I5" t="n">
-        <v>38.611</v>
+        <v>7410.386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>